<commit_message>
traduccion de los jugadores historico conseguida
</commit_message>
<xml_diff>
--- a/data/split.xlsx
+++ b/data/split.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>split</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -462,6 +467,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -475,6 +485,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2022 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -488,6 +503,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2022 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -501,6 +521,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2021 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -514,6 +539,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2021 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -527,6 +557,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2020 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -540,6 +575,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2020 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -553,6 +593,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2019 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -566,6 +611,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2019 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -579,6 +629,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2018 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -592,6 +647,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2018 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -605,6 +665,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2017 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -618,6 +683,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2016 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -631,6 +701,11 @@
           <t>Spring</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2016 Spring</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -644,6 +719,11 @@
           <t>Summer</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2015 Summer</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -655,6 +735,29 @@
       <c r="C17" t="inlineStr">
         <is>
           <t>Spring</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2015 Spring</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Summer</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2023 Summer</t>
         </is>
       </c>
     </row>

</xml_diff>